<commit_message>
Add wk 7 PR
</commit_message>
<xml_diff>
--- a/PR/Week07_Risk_Defect_F19a_T04.xlsx
+++ b/PR/Week07_Risk_Defect_F19a_T04.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akankshadiwedy/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292F3123-29E0-6841-85A8-73F45CCB1C57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8908B2-5A0A-2741-8677-D90230E65270}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="502" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="502" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Risk" sheetId="1" r:id="rId1"/>
@@ -177,9 +177,6 @@
     <t>Team members met frequently to restructure the architecture by discussing the possibilities</t>
   </si>
   <si>
-    <t>Top Project Risks as of 10/23/2019</t>
-  </si>
-  <si>
     <t>Team members are actively learning to work with React and Django and development is going as planned</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>Process the output data from backend to meet the requirements of frontend input format.</t>
+  </si>
+  <si>
+    <t>Top Project Risks as of 11/06/2019</t>
   </si>
 </sst>
 </file>
@@ -982,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:K994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1001,7 +1001,7 @@
   <sheetData>
     <row r="2" spans="2:11" ht="14" x14ac:dyDescent="0.15">
       <c r="B2" s="51" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C2" s="52"/>
       <c r="D2" s="52"/>
@@ -1110,7 +1110,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K7" s="18">
         <v>4</v>
@@ -1143,7 +1143,7 @@
         <v>8</v>
       </c>
       <c r="J8" s="45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K8" s="34">
         <v>5</v>
@@ -1176,7 +1176,7 @@
         <v>28</v>
       </c>
       <c r="J9" s="45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K9" s="34">
         <v>5</v>
@@ -1209,7 +1209,7 @@
         <v>6</v>
       </c>
       <c r="J10" s="46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K10" s="44">
         <v>5</v>
@@ -2217,7 +2217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -2560,10 +2560,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>

</xml_diff>